<commit_message>
$$ to ##. Working version of script update.ps1
</commit_message>
<xml_diff>
--- a/src/NewEngineFormulas.xlsx
+++ b/src/NewEngineFormulas.xlsx
@@ -165,9 +165,6 @@
     <t>Factory Lvl</t>
   </si>
   <si>
-    <t>New Disc Lvl</t>
-  </si>
-  <si>
     <t>cursor8_310hp.sii</t>
   </si>
   <si>
@@ -400,6 +397,9 @@
   </si>
   <si>
     <t>TempKeyHP</t>
+  </si>
+  <si>
+    <t>New Lvl</t>
   </si>
 </sst>
 </file>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +960,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2"/>
@@ -981,13 +981,13 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1169,13 +1169,13 @@
         <v>39</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>48</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="16">
-        <f>ROUNDDOWN(((F25-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H25:H32" si="1">ROUNDDOWN(((F25-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>7</v>
       </c>
     </row>
@@ -1315,14 +1315,14 @@
         <v>410</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ref="F26:F32" si="1">($E$24+B26)*(IF(B26&lt;=$C$8,1,0)*$D$8+IF(AND(B26&gt;$C$8,B26&lt;=$C$9),1,0)*$D$9+IF(AND(B26&gt;$C$9,B26&lt;=$C$10),1,0)*$D$10+IF(AND(B26&gt;$C$10,B26&lt;=$C$11),1,0)*$D$11+IF(AND(B26&gt;$C$11,B26&lt;=$C$12),1,0)*$D$12+IF(AND(B26&gt;$C$12,B26&lt;=$C$13),1,0)*$D$13+IF(AND(B26&gt;$C$13,B26&lt;=$C$14),1,0)*$D$14+IF(AND(B26&gt;$C$14,B26&lt;=$C$15),1,0)*$D$15+IF(AND(B26&gt;$C$15,B26&lt;=$C$16),1,0)*$D$16+IF(AND(B26&gt;$C$16,B26&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F26:F32" si="2">($E$24+B26)*(IF(B26&lt;=$C$8,1,0)*$D$8+IF(AND(B26&gt;$C$8,B26&lt;=$C$9),1,0)*$D$9+IF(AND(B26&gt;$C$9,B26&lt;=$C$10),1,0)*$D$10+IF(AND(B26&gt;$C$10,B26&lt;=$C$11),1,0)*$D$11+IF(AND(B26&gt;$C$11,B26&lt;=$C$12),1,0)*$D$12+IF(AND(B26&gt;$C$12,B26&lt;=$C$13),1,0)*$D$13+IF(AND(B26&gt;$C$13,B26&lt;=$C$14),1,0)*$D$14+IF(AND(B26&gt;$C$14,B26&lt;=$C$15),1,0)*$D$15+IF(AND(B26&gt;$C$15,B26&lt;=$C$16),1,0)*$D$16+IF(AND(B26&gt;$C$16,B26&lt;=$C$17),1,0)*$D$17)</f>
         <v>1504</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
       </c>
       <c r="H26" s="16">
-        <f>ROUNDDOWN(((F26-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -1334,14 +1334,14 @@
         <v>435</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2316</v>
       </c>
       <c r="G27" s="1">
         <v>6</v>
       </c>
       <c r="H27" s="16">
-        <f>ROUNDDOWN(((F27-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1353,14 +1353,14 @@
         <v>450</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2352</v>
       </c>
       <c r="G28" s="1">
         <v>8</v>
       </c>
       <c r="H28" s="16">
-        <f>ROUNDDOWN(((F28-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1372,14 +1372,14 @@
         <v>460</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2970</v>
       </c>
       <c r="G29" s="1">
         <v>10</v>
       </c>
       <c r="H29" s="16">
-        <f>ROUNDDOWN(((F29-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1391,14 +1391,14 @@
         <v>480</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3030</v>
       </c>
       <c r="G30" s="1">
         <v>14</v>
       </c>
       <c r="H30" s="16">
-        <f>ROUNDDOWN(((F30-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1410,14 +1410,14 @@
         <v>510</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3328</v>
       </c>
       <c r="G31" s="1">
         <v>16</v>
       </c>
       <c r="H31" s="16">
-        <f>ROUNDDOWN(((F31-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
@@ -1429,14 +1429,14 @@
         <v>530</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3392</v>
       </c>
       <c r="G32" s="1">
         <v>18</v>
       </c>
       <c r="H32" s="16">
-        <f>ROUNDDOWN(((F32-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
@@ -1472,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="16">
-        <f>ROUNDDOWN(((F34-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H34:H41" si="3">ROUNDDOWN(((F34-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
@@ -1484,14 +1484,14 @@
         <v>330</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" ref="F35:F41" si="2">($E$33+B35)*(IF(B35&lt;=$C$8,1,0)*$D$8+IF(AND(B35&gt;$C$8,B35&lt;=$C$9),1,0)*$D$9+IF(AND(B35&gt;$C$9,B35&lt;=$C$10),1,0)*$D$10+IF(AND(B35&gt;$C$10,B35&lt;=$C$11),1,0)*$D$11+IF(AND(B35&gt;$C$11,B35&lt;=$C$12),1,0)*$D$12+IF(AND(B35&gt;$C$12,B35&lt;=$C$13),1,0)*$D$13+IF(AND(B35&gt;$C$13,B35&lt;=$C$14),1,0)*$D$14+IF(AND(B35&gt;$C$14,B35&lt;=$C$15),1,0)*$D$15+IF(AND(B35&gt;$C$15,B35&lt;=$C$16),1,0)*$D$16+IF(AND(B35&gt;$C$16,B35&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F35:F41" si="4">($E$33+B35)*(IF(B35&lt;=$C$8,1,0)*$D$8+IF(AND(B35&gt;$C$8,B35&lt;=$C$9),1,0)*$D$9+IF(AND(B35&gt;$C$9,B35&lt;=$C$10),1,0)*$D$10+IF(AND(B35&gt;$C$10,B35&lt;=$C$11),1,0)*$D$11+IF(AND(B35&gt;$C$11,B35&lt;=$C$12),1,0)*$D$12+IF(AND(B35&gt;$C$12,B35&lt;=$C$13),1,0)*$D$13+IF(AND(B35&gt;$C$13,B35&lt;=$C$14),1,0)*$D$14+IF(AND(B35&gt;$C$14,B35&lt;=$C$15),1,0)*$D$15+IF(AND(B35&gt;$C$15,B35&lt;=$C$16),1,0)*$D$16+IF(AND(B35&gt;$C$16,B35&lt;=$C$17),1,0)*$D$17)</f>
         <v>356</v>
       </c>
       <c r="G35" s="1">
         <v>6</v>
       </c>
       <c r="H35" s="16">
-        <f>ROUNDDOWN(((F35-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1503,14 +1503,14 @@
         <v>360</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>736</v>
       </c>
       <c r="G36" s="1">
         <v>8</v>
       </c>
       <c r="H36" s="16">
-        <f>ROUNDDOWN(((F36-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1522,14 +1522,14 @@
         <v>400</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1536</v>
       </c>
       <c r="G37" s="1">
         <v>9</v>
       </c>
       <c r="H37" s="16">
-        <f>ROUNDDOWN(((F37-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
@@ -1541,14 +1541,14 @@
         <v>420</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1568</v>
       </c>
       <c r="G38" s="1">
         <v>10</v>
       </c>
       <c r="H38" s="16">
-        <f>ROUNDDOWN(((F38-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
@@ -1560,14 +1560,14 @@
         <v>460</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3060</v>
       </c>
       <c r="G39" s="1">
         <v>12</v>
       </c>
       <c r="H39" s="16">
-        <f>ROUNDDOWN(((F39-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
@@ -1579,14 +1579,14 @@
         <v>500</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3180</v>
       </c>
       <c r="G40" s="1">
         <v>14</v>
       </c>
       <c r="H40" s="16">
-        <f>ROUNDDOWN(((F40-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -1598,14 +1598,14 @@
         <v>560</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3696</v>
       </c>
       <c r="G41" s="1">
         <v>16</v>
       </c>
       <c r="H41" s="16">
-        <f>ROUNDDOWN(((F41-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1">
         <v>310</v>
@@ -1641,83 +1641,83 @@
         <v>0</v>
       </c>
       <c r="H43" s="16">
-        <f>ROUNDDOWN(((F43-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H43:H49" si="5">ROUNDDOWN(((F43-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1">
         <v>330</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" ref="F44:F49" si="3">($E$42+B44)*(IF(B44&lt;=$C$8,1,0)*$D$8+IF(AND(B44&gt;$C$8,B44&lt;=$C$9),1,0)*$D$9+IF(AND(B44&gt;$C$9,B44&lt;=$C$10),1,0)*$D$10+IF(AND(B44&gt;$C$10,B44&lt;=$C$11),1,0)*$D$11+IF(AND(B44&gt;$C$11,B44&lt;=$C$12),1,0)*$D$12+IF(AND(B44&gt;$C$12,B44&lt;=$C$13),1,0)*$D$13+IF(AND(B44&gt;$C$13,B44&lt;=$C$14),1,0)*$D$14+IF(AND(B44&gt;$C$14,B44&lt;=$C$15),1,0)*$D$15+IF(AND(B44&gt;$C$15,B44&lt;=$C$16),1,0)*$D$16+IF(AND(B44&gt;$C$16,B44&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F44:F49" si="6">($E$42+B44)*(IF(B44&lt;=$C$8,1,0)*$D$8+IF(AND(B44&gt;$C$8,B44&lt;=$C$9),1,0)*$D$9+IF(AND(B44&gt;$C$9,B44&lt;=$C$10),1,0)*$D$10+IF(AND(B44&gt;$C$10,B44&lt;=$C$11),1,0)*$D$11+IF(AND(B44&gt;$C$11,B44&lt;=$C$12),1,0)*$D$12+IF(AND(B44&gt;$C$12,B44&lt;=$C$13),1,0)*$D$13+IF(AND(B44&gt;$C$13,B44&lt;=$C$14),1,0)*$D$14+IF(AND(B44&gt;$C$14,B44&lt;=$C$15),1,0)*$D$15+IF(AND(B44&gt;$C$15,B44&lt;=$C$16),1,0)*$D$16+IF(AND(B44&gt;$C$16,B44&lt;=$C$17),1,0)*$D$17)</f>
         <v>356</v>
       </c>
       <c r="G44" s="1">
         <v>6</v>
       </c>
       <c r="H44" s="16">
-        <f>ROUNDDOWN(((F44-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1">
         <v>360</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>736</v>
       </c>
       <c r="G45" s="1">
         <v>8</v>
       </c>
       <c r="H45" s="16">
-        <f>ROUNDDOWN(((F45-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1">
         <v>420</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1568</v>
       </c>
       <c r="G46" s="1">
         <v>10</v>
       </c>
       <c r="H46" s="16">
-        <f>ROUNDDOWN(((F46-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1">
         <v>450</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2424</v>
       </c>
       <c r="G47" s="1">
         <v>12</v>
       </c>
       <c r="H47" s="16">
-        <f>ROUNDDOWN(((F47-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
@@ -1729,14 +1729,14 @@
         <v>500</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3180</v>
       </c>
       <c r="G48" s="1">
         <v>14</v>
       </c>
       <c r="H48" s="16">
-        <f>ROUNDDOWN(((F48-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -1748,14 +1748,14 @@
         <v>560</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3696</v>
       </c>
       <c r="G49" s="1">
         <v>16</v>
       </c>
       <c r="H49" s="16">
-        <f>ROUNDDOWN(((F49-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1">
         <v>320</v>
@@ -1791,121 +1791,121 @@
         <v>0</v>
       </c>
       <c r="H51" s="16">
-        <f>ROUNDDOWN(((F51-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H51:H57" si="7">ROUNDDOWN(((F51-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" s="1">
         <v>360</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" ref="F52:F57" si="4">($E$50+B52)*(IF(B52&lt;=$C$8,1,0)*$D$8+IF(AND(B52&gt;$C$8,B52&lt;=$C$9),1,0)*$D$9+IF(AND(B52&gt;$C$9,B52&lt;=$C$10),1,0)*$D$10+IF(AND(B52&gt;$C$10,B52&lt;=$C$11),1,0)*$D$11+IF(AND(B52&gt;$C$11,B52&lt;=$C$12),1,0)*$D$12+IF(AND(B52&gt;$C$12,B52&lt;=$C$13),1,0)*$D$13+IF(AND(B52&gt;$C$13,B52&lt;=$C$14),1,0)*$D$14+IF(AND(B52&gt;$C$14,B52&lt;=$C$15),1,0)*$D$15+IF(AND(B52&gt;$C$15,B52&lt;=$C$16),1,0)*$D$16+IF(AND(B52&gt;$C$16,B52&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F52:F57" si="8">($E$50+B52)*(IF(B52&lt;=$C$8,1,0)*$D$8+IF(AND(B52&gt;$C$8,B52&lt;=$C$9),1,0)*$D$9+IF(AND(B52&gt;$C$9,B52&lt;=$C$10),1,0)*$D$10+IF(AND(B52&gt;$C$10,B52&lt;=$C$11),1,0)*$D$11+IF(AND(B52&gt;$C$11,B52&lt;=$C$12),1,0)*$D$12+IF(AND(B52&gt;$C$12,B52&lt;=$C$13),1,0)*$D$13+IF(AND(B52&gt;$C$13,B52&lt;=$C$14),1,0)*$D$14+IF(AND(B52&gt;$C$14,B52&lt;=$C$15),1,0)*$D$15+IF(AND(B52&gt;$C$15,B52&lt;=$C$16),1,0)*$D$16+IF(AND(B52&gt;$C$16,B52&lt;=$C$17),1,0)*$D$17)</f>
         <v>832</v>
       </c>
       <c r="G52" s="1">
         <v>6</v>
       </c>
       <c r="H52" s="16">
-        <f>ROUNDDOWN(((F52-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" s="1">
         <v>400</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1728</v>
       </c>
       <c r="G53" s="1">
         <v>8</v>
       </c>
       <c r="H53" s="16">
-        <f>ROUNDDOWN(((F53-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" s="1">
         <v>440</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2688</v>
       </c>
       <c r="G54" s="1">
         <v>10</v>
       </c>
       <c r="H54" s="16">
-        <f>ROUNDDOWN(((F54-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="1">
         <v>480</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3480</v>
       </c>
       <c r="G55" s="1">
         <v>12</v>
       </c>
       <c r="H55" s="16">
-        <f>ROUNDDOWN(((F55-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1">
         <v>540</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3904</v>
       </c>
       <c r="G56" s="1">
         <v>14</v>
       </c>
       <c r="H56" s="16">
-        <f>ROUNDDOWN(((F56-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1">
         <v>680</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4760</v>
       </c>
       <c r="G57" s="1">
         <v>16</v>
       </c>
       <c r="H57" s="16">
-        <f>ROUNDDOWN(((F57-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
     </row>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B59" s="1">
         <v>360</v>
@@ -1941,121 +1941,121 @@
         <v>0</v>
       </c>
       <c r="H59" s="16">
-        <f>ROUNDDOWN(((F59-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H59:H65" si="9">ROUNDDOWN(((F59-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1">
         <v>400</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" ref="F60:F65" si="5">($E$58+B60)*(IF(B60&lt;=$C$8,1,0)*$D$8+IF(AND(B60&gt;$C$8,B60&lt;=$C$9),1,0)*$D$9+IF(AND(B60&gt;$C$9,B60&lt;=$C$10),1,0)*$D$10+IF(AND(B60&gt;$C$10,B60&lt;=$C$11),1,0)*$D$11+IF(AND(B60&gt;$C$11,B60&lt;=$C$12),1,0)*$D$12+IF(AND(B60&gt;$C$12,B60&lt;=$C$13),1,0)*$D$13+IF(AND(B60&gt;$C$13,B60&lt;=$C$14),1,0)*$D$14+IF(AND(B60&gt;$C$14,B60&lt;=$C$15),1,0)*$D$15+IF(AND(B60&gt;$C$15,B60&lt;=$C$16),1,0)*$D$16+IF(AND(B60&gt;$C$16,B60&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F60:F65" si="10">($E$58+B60)*(IF(B60&lt;=$C$8,1,0)*$D$8+IF(AND(B60&gt;$C$8,B60&lt;=$C$9),1,0)*$D$9+IF(AND(B60&gt;$C$9,B60&lt;=$C$10),1,0)*$D$10+IF(AND(B60&gt;$C$10,B60&lt;=$C$11),1,0)*$D$11+IF(AND(B60&gt;$C$11,B60&lt;=$C$12),1,0)*$D$12+IF(AND(B60&gt;$C$12,B60&lt;=$C$13),1,0)*$D$13+IF(AND(B60&gt;$C$13,B60&lt;=$C$14),1,0)*$D$14+IF(AND(B60&gt;$C$14,B60&lt;=$C$15),1,0)*$D$15+IF(AND(B60&gt;$C$15,B60&lt;=$C$16),1,0)*$D$16+IF(AND(B60&gt;$C$16,B60&lt;=$C$17),1,0)*$D$17)</f>
         <v>1664</v>
       </c>
       <c r="G60" s="1">
         <v>6</v>
       </c>
       <c r="H60" s="16">
-        <f>ROUNDDOWN(((F60-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="1">
         <v>440</v>
       </c>
       <c r="F61" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2592</v>
       </c>
       <c r="G61" s="1">
         <v>8</v>
       </c>
       <c r="H61" s="16">
-        <f>ROUNDDOWN(((F61-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="1">
         <v>480</v>
       </c>
       <c r="F62" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3360</v>
       </c>
       <c r="G62" s="1">
         <v>12</v>
       </c>
       <c r="H62" s="16">
-        <f>ROUNDDOWN(((F62-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1">
         <v>520</v>
       </c>
       <c r="F63" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3712</v>
       </c>
       <c r="G63" s="1">
         <v>16</v>
       </c>
       <c r="H63" s="16">
-        <f>ROUNDDOWN(((F63-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1">
         <v>560</v>
       </c>
       <c r="F64" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3960</v>
       </c>
       <c r="G64" s="1">
         <v>18</v>
       </c>
       <c r="H64" s="16">
-        <f>ROUNDDOWN(((F64-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1">
         <v>640</v>
       </c>
       <c r="F65" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4352</v>
       </c>
       <c r="G65" s="1">
         <v>20</v>
       </c>
       <c r="H65" s="16">
-        <f>ROUNDDOWN(((F65-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1">
         <v>320</v>
@@ -2091,159 +2091,159 @@
         <v>0</v>
       </c>
       <c r="H67" s="16">
-        <f>ROUNDDOWN(((F67-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H67:H75" si="11">ROUNDDOWN(((F67-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="1">
         <v>360</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" ref="F68:F75" si="6">($E$66+B68)*(IF(B68&lt;=$C$8,1,0)*$D$8+IF(AND(B68&gt;$C$8,B68&lt;=$C$9),1,0)*$D$9+IF(AND(B68&gt;$C$9,B68&lt;=$C$10),1,0)*$D$10+IF(AND(B68&gt;$C$10,B68&lt;=$C$11),1,0)*$D$11+IF(AND(B68&gt;$C$11,B68&lt;=$C$12),1,0)*$D$12+IF(AND(B68&gt;$C$12,B68&lt;=$C$13),1,0)*$D$13+IF(AND(B68&gt;$C$13,B68&lt;=$C$14),1,0)*$D$14+IF(AND(B68&gt;$C$14,B68&lt;=$C$15),1,0)*$D$15+IF(AND(B68&gt;$C$15,B68&lt;=$C$16),1,0)*$D$16+IF(AND(B68&gt;$C$16,B68&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F68:F75" si="12">($E$66+B68)*(IF(B68&lt;=$C$8,1,0)*$D$8+IF(AND(B68&gt;$C$8,B68&lt;=$C$9),1,0)*$D$9+IF(AND(B68&gt;$C$9,B68&lt;=$C$10),1,0)*$D$10+IF(AND(B68&gt;$C$10,B68&lt;=$C$11),1,0)*$D$11+IF(AND(B68&gt;$C$11,B68&lt;=$C$12),1,0)*$D$12+IF(AND(B68&gt;$C$12,B68&lt;=$C$13),1,0)*$D$13+IF(AND(B68&gt;$C$13,B68&lt;=$C$14),1,0)*$D$14+IF(AND(B68&gt;$C$14,B68&lt;=$C$15),1,0)*$D$15+IF(AND(B68&gt;$C$15,B68&lt;=$C$16),1,0)*$D$16+IF(AND(B68&gt;$C$16,B68&lt;=$C$17),1,0)*$D$17)</f>
         <v>766.40000000000009</v>
       </c>
       <c r="G68" s="1">
         <v>6</v>
       </c>
       <c r="H68" s="16">
-        <f>ROUNDDOWN(((F68-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="1">
         <v>408</v>
       </c>
       <c r="F69" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>1609.6000000000001</v>
       </c>
       <c r="G69" s="1">
         <v>8</v>
       </c>
       <c r="H69" s="16">
-        <f>ROUNDDOWN(((F69-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="1">
         <v>435</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>2479.1999999999998</v>
       </c>
       <c r="G70" s="1">
         <v>10</v>
       </c>
       <c r="H70" s="16">
-        <f>ROUNDDOWN(((F70-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="1">
         <v>456</v>
       </c>
       <c r="F71" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3162</v>
       </c>
       <c r="G71" s="1">
         <v>12</v>
       </c>
       <c r="H71" s="16">
-        <f>ROUNDDOWN(((F71-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1">
         <v>476</v>
       </c>
       <c r="F72" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3222</v>
       </c>
       <c r="G72" s="1">
         <v>14</v>
       </c>
       <c r="H72" s="16">
-        <f>ROUNDDOWN(((F72-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1">
         <v>510</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3545.6000000000004</v>
       </c>
       <c r="G73" s="1">
         <v>16</v>
       </c>
       <c r="H73" s="16">
-        <f>ROUNDDOWN(((F73-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="1">
         <v>551</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3791.7</v>
       </c>
       <c r="G74" s="1">
         <v>18</v>
       </c>
       <c r="H74" s="16">
-        <f>ROUNDDOWN(((F74-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="1">
         <v>598</v>
       </c>
       <c r="F75" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3946.7999999999997</v>
       </c>
       <c r="G75" s="1">
         <v>20</v>
       </c>
       <c r="H75" s="16">
-        <f>ROUNDDOWN(((F75-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
     </row>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="1">
         <v>421</v>
@@ -2279,121 +2279,121 @@
         <v>0</v>
       </c>
       <c r="H77" s="16">
-        <f>ROUNDDOWN(((F77-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H77:H83" si="13">ROUNDDOWN(((F77-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1">
         <v>449</v>
       </c>
       <c r="F78" s="1">
-        <f t="shared" ref="F78:F83" si="7">($E$76+B78)*(IF(B78&lt;=$C$8,1,0)*$D$8+IF(AND(B78&gt;$C$8,B78&lt;=$C$9),1,0)*$D$9+IF(AND(B78&gt;$C$9,B78&lt;=$C$10),1,0)*$D$10+IF(AND(B78&gt;$C$10,B78&lt;=$C$11),1,0)*$D$11+IF(AND(B78&gt;$C$11,B78&lt;=$C$12),1,0)*$D$12+IF(AND(B78&gt;$C$12,B78&lt;=$C$13),1,0)*$D$13+IF(AND(B78&gt;$C$13,B78&lt;=$C$14),1,0)*$D$14+IF(AND(B78&gt;$C$14,B78&lt;=$C$15),1,0)*$D$15+IF(AND(B78&gt;$C$15,B78&lt;=$C$16),1,0)*$D$16+IF(AND(B78&gt;$C$16,B78&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F78:F83" si="14">($E$76+B78)*(IF(B78&lt;=$C$8,1,0)*$D$8+IF(AND(B78&gt;$C$8,B78&lt;=$C$9),1,0)*$D$9+IF(AND(B78&gt;$C$9,B78&lt;=$C$10),1,0)*$D$10+IF(AND(B78&gt;$C$10,B78&lt;=$C$11),1,0)*$D$11+IF(AND(B78&gt;$C$11,B78&lt;=$C$12),1,0)*$D$12+IF(AND(B78&gt;$C$12,B78&lt;=$C$13),1,0)*$D$13+IF(AND(B78&gt;$C$13,B78&lt;=$C$14),1,0)*$D$14+IF(AND(B78&gt;$C$14,B78&lt;=$C$15),1,0)*$D$15+IF(AND(B78&gt;$C$15,B78&lt;=$C$16),1,0)*$D$16+IF(AND(B78&gt;$C$16,B78&lt;=$C$17),1,0)*$D$17)</f>
         <v>2577.6</v>
       </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
       <c r="H78" s="16">
-        <f>ROUNDDOWN(((F78-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1">
         <v>476</v>
       </c>
       <c r="F79" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>3303</v>
       </c>
       <c r="G79" s="1">
         <v>10</v>
       </c>
       <c r="H79" s="16">
-        <f>ROUNDDOWN(((F79-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1">
         <v>510</v>
       </c>
       <c r="F80" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>3632</v>
       </c>
       <c r="G80" s="1">
         <v>12</v>
       </c>
       <c r="H80" s="16">
-        <f>ROUNDDOWN(((F80-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="1">
         <v>517</v>
       </c>
       <c r="F81" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>3654.4</v>
       </c>
       <c r="G81" s="1">
         <v>14</v>
       </c>
       <c r="H81" s="16">
-        <f>ROUNDDOWN(((F81-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1">
         <v>578</v>
       </c>
       <c r="F82" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>3969.8999999999996</v>
       </c>
       <c r="G82" s="1">
         <v>16</v>
       </c>
       <c r="H82" s="16">
-        <f>ROUNDDOWN(((F82-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="1">
         <v>625</v>
       </c>
       <c r="F83" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>4250</v>
       </c>
       <c r="G83" s="1">
         <v>20</v>
       </c>
       <c r="H83" s="16">
-        <f>ROUNDDOWN(((F83-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="85" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="1">
         <v>440</v>
@@ -2435,13 +2435,13 @@
     </row>
     <row r="86" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" s="1">
         <v>480</v>
       </c>
       <c r="F86" s="1">
-        <f t="shared" ref="F86:F87" si="8">($E$84+B86)*(IF(B86&lt;=$C$8,1,0)*$D$8+IF(AND(B86&gt;$C$8,B86&lt;=$C$9),1,0)*$D$9+IF(AND(B86&gt;$C$9,B86&lt;=$C$10),1,0)*$D$10+IF(AND(B86&gt;$C$10,B86&lt;=$C$11),1,0)*$D$11+IF(AND(B86&gt;$C$11,B86&lt;=$C$12),1,0)*$D$12+IF(AND(B86&gt;$C$12,B86&lt;=$C$13),1,0)*$D$13+IF(AND(B86&gt;$C$13,B86&lt;=$C$14),1,0)*$D$14+IF(AND(B86&gt;$C$14,B86&lt;=$C$15),1,0)*$D$15+IF(AND(B86&gt;$C$15,B86&lt;=$C$16),1,0)*$D$16+IF(AND(B86&gt;$C$16,B86&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F86:F87" si="15">($E$84+B86)*(IF(B86&lt;=$C$8,1,0)*$D$8+IF(AND(B86&gt;$C$8,B86&lt;=$C$9),1,0)*$D$9+IF(AND(B86&gt;$C$9,B86&lt;=$C$10),1,0)*$D$10+IF(AND(B86&gt;$C$10,B86&lt;=$C$11),1,0)*$D$11+IF(AND(B86&gt;$C$11,B86&lt;=$C$12),1,0)*$D$12+IF(AND(B86&gt;$C$12,B86&lt;=$C$13),1,0)*$D$13+IF(AND(B86&gt;$C$13,B86&lt;=$C$14),1,0)*$D$14+IF(AND(B86&gt;$C$14,B86&lt;=$C$15),1,0)*$D$15+IF(AND(B86&gt;$C$15,B86&lt;=$C$16),1,0)*$D$16+IF(AND(B86&gt;$C$16,B86&lt;=$C$17),1,0)*$D$17)</f>
         <v>3000</v>
       </c>
       <c r="G86" s="1">
@@ -2454,13 +2454,13 @@
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="1">
         <v>520</v>
       </c>
       <c r="F87" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>3328</v>
       </c>
       <c r="G87" s="1">
@@ -2490,7 +2490,7 @@
     </row>
     <row r="89" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89" s="1">
         <v>380</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="90" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B90" s="1">
         <v>430</v>
       </c>
       <c r="F90" s="1">
-        <f t="shared" ref="F90:F91" si="9">($E$88+B90)*(IF(B90&lt;=$C$8,1,0)*$D$8+IF(AND(B90&gt;$C$8,B90&lt;=$C$9),1,0)*$D$9+IF(AND(B90&gt;$C$9,B90&lt;=$C$10),1,0)*$D$10+IF(AND(B90&gt;$C$10,B90&lt;=$C$11),1,0)*$D$11+IF(AND(B90&gt;$C$11,B90&lt;=$C$12),1,0)*$D$12+IF(AND(B90&gt;$C$12,B90&lt;=$C$13),1,0)*$D$13+IF(AND(B90&gt;$C$13,B90&lt;=$C$14),1,0)*$D$14+IF(AND(B90&gt;$C$14,B90&lt;=$C$15),1,0)*$D$15+IF(AND(B90&gt;$C$15,B90&lt;=$C$16),1,0)*$D$16+IF(AND(B90&gt;$C$16,B90&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F90:F91" si="16">($E$88+B90)*(IF(B90&lt;=$C$8,1,0)*$D$8+IF(AND(B90&gt;$C$8,B90&lt;=$C$9),1,0)*$D$9+IF(AND(B90&gt;$C$9,B90&lt;=$C$10),1,0)*$D$10+IF(AND(B90&gt;$C$10,B90&lt;=$C$11),1,0)*$D$11+IF(AND(B90&gt;$C$11,B90&lt;=$C$12),1,0)*$D$12+IF(AND(B90&gt;$C$12,B90&lt;=$C$13),1,0)*$D$13+IF(AND(B90&gt;$C$13,B90&lt;=$C$14),1,0)*$D$14+IF(AND(B90&gt;$C$14,B90&lt;=$C$15),1,0)*$D$15+IF(AND(B90&gt;$C$15,B90&lt;=$C$16),1,0)*$D$16+IF(AND(B90&gt;$C$16,B90&lt;=$C$17),1,0)*$D$17)</f>
         <v>2136</v>
       </c>
       <c r="G90" s="1">
@@ -2528,13 +2528,13 @@
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="1">
         <v>460</v>
       </c>
       <c r="F91" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2760</v>
       </c>
       <c r="G91" s="1">
@@ -2564,7 +2564,7 @@
     </row>
     <row r="93" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B93" s="1">
         <v>380</v>
@@ -2577,102 +2577,102 @@
         <v>0</v>
       </c>
       <c r="H93" s="16">
-        <f>ROUNDDOWN(((F93-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H93:H98" si="17">ROUNDDOWN(((F93-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B94" s="1">
         <v>430</v>
       </c>
       <c r="F94" s="1">
-        <f t="shared" ref="F94:F98" si="10">($E$92+B94)*(IF(B94&lt;=$C$8,1,0)*$D$8+IF(AND(B94&gt;$C$8,B94&lt;=$C$9),1,0)*$D$9+IF(AND(B94&gt;$C$9,B94&lt;=$C$10),1,0)*$D$10+IF(AND(B94&gt;$C$10,B94&lt;=$C$11),1,0)*$D$11+IF(AND(B94&gt;$C$11,B94&lt;=$C$12),1,0)*$D$12+IF(AND(B94&gt;$C$12,B94&lt;=$C$13),1,0)*$D$13+IF(AND(B94&gt;$C$13,B94&lt;=$C$14),1,0)*$D$14+IF(AND(B94&gt;$C$14,B94&lt;=$C$15),1,0)*$D$15+IF(AND(B94&gt;$C$15,B94&lt;=$C$16),1,0)*$D$16+IF(AND(B94&gt;$C$16,B94&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F94:F98" si="18">($E$92+B94)*(IF(B94&lt;=$C$8,1,0)*$D$8+IF(AND(B94&gt;$C$8,B94&lt;=$C$9),1,0)*$D$9+IF(AND(B94&gt;$C$9,B94&lt;=$C$10),1,0)*$D$10+IF(AND(B94&gt;$C$10,B94&lt;=$C$11),1,0)*$D$11+IF(AND(B94&gt;$C$11,B94&lt;=$C$12),1,0)*$D$12+IF(AND(B94&gt;$C$12,B94&lt;=$C$13),1,0)*$D$13+IF(AND(B94&gt;$C$13,B94&lt;=$C$14),1,0)*$D$14+IF(AND(B94&gt;$C$14,B94&lt;=$C$15),1,0)*$D$15+IF(AND(B94&gt;$C$15,B94&lt;=$C$16),1,0)*$D$16+IF(AND(B94&gt;$C$16,B94&lt;=$C$17),1,0)*$D$17)</f>
         <v>2280</v>
       </c>
       <c r="G94" s="1">
         <v>10</v>
       </c>
       <c r="H94" s="16">
-        <f>ROUNDDOWN(((F94-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B95" s="1">
         <v>440</v>
       </c>
       <c r="F95" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>2304</v>
       </c>
       <c r="G95" s="1">
         <v>12</v>
       </c>
       <c r="H95" s="16">
-        <f>ROUNDDOWN(((F95-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B96" s="1">
         <v>460</v>
       </c>
       <c r="F96" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>2940</v>
       </c>
       <c r="G96" s="1">
         <v>14</v>
       </c>
       <c r="H96" s="16">
-        <f>ROUNDDOWN(((F96-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="17"/>
         <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" s="1">
         <v>480</v>
       </c>
       <c r="F97" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3000</v>
       </c>
       <c r="G97" s="1">
         <v>16</v>
       </c>
       <c r="H97" s="16">
-        <f>ROUNDDOWN(((F97-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="17"/>
         <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" s="1">
         <v>520</v>
       </c>
       <c r="F98" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3328</v>
       </c>
       <c r="G98" s="1">
         <v>18</v>
       </c>
       <c r="H98" s="16">
-        <f>ROUNDDOWN(((F98-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="17"/>
         <v>21</v>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="100" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B100" s="1">
         <v>360</v>
@@ -2708,216 +2708,216 @@
         <v>0</v>
       </c>
       <c r="H100" s="16">
-        <f>ROUNDDOWN(((F100-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H100:H111" si="19">ROUNDDOWN(((F100-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B101" s="1">
         <v>380</v>
       </c>
       <c r="F101" s="1">
-        <f t="shared" ref="F101:F111" si="11">($E$99+B101)*(IF(B101&lt;=$C$8,1,0)*$D$8+IF(AND(B101&gt;$C$8,B101&lt;=$C$9),1,0)*$D$9+IF(AND(B101&gt;$C$9,B101&lt;=$C$10),1,0)*$D$10+IF(AND(B101&gt;$C$10,B101&lt;=$C$11),1,0)*$D$11+IF(AND(B101&gt;$C$11,B101&lt;=$C$12),1,0)*$D$12+IF(AND(B101&gt;$C$12,B101&lt;=$C$13),1,0)*$D$13+IF(AND(B101&gt;$C$13,B101&lt;=$C$14),1,0)*$D$14+IF(AND(B101&gt;$C$14,B101&lt;=$C$15),1,0)*$D$15+IF(AND(B101&gt;$C$15,B101&lt;=$C$16),1,0)*$D$16+IF(AND(B101&gt;$C$16,B101&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F101:F111" si="20">($E$99+B101)*(IF(B101&lt;=$C$8,1,0)*$D$8+IF(AND(B101&gt;$C$8,B101&lt;=$C$9),1,0)*$D$9+IF(AND(B101&gt;$C$9,B101&lt;=$C$10),1,0)*$D$10+IF(AND(B101&gt;$C$10,B101&lt;=$C$11),1,0)*$D$11+IF(AND(B101&gt;$C$11,B101&lt;=$C$12),1,0)*$D$12+IF(AND(B101&gt;$C$12,B101&lt;=$C$13),1,0)*$D$13+IF(AND(B101&gt;$C$13,B101&lt;=$C$14),1,0)*$D$14+IF(AND(B101&gt;$C$14,B101&lt;=$C$15),1,0)*$D$15+IF(AND(B101&gt;$C$15,B101&lt;=$C$16),1,0)*$D$16+IF(AND(B101&gt;$C$16,B101&lt;=$C$17),1,0)*$D$17)</f>
         <v>1776</v>
       </c>
       <c r="G101" s="1">
         <v>8</v>
       </c>
       <c r="H101" s="16">
-        <f>ROUNDDOWN(((F101-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B102" s="1">
         <v>400</v>
       </c>
       <c r="F102" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>1808</v>
       </c>
       <c r="G102" s="1">
         <v>8</v>
       </c>
       <c r="H102" s="16">
-        <f>ROUNDDOWN(((F102-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B103" s="1">
         <v>420</v>
       </c>
       <c r="F103" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>1840</v>
       </c>
       <c r="G103" s="1">
         <v>10</v>
       </c>
       <c r="H103" s="16">
-        <f>ROUNDDOWN(((F103-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B104" s="1">
         <v>440</v>
       </c>
       <c r="F104" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2808</v>
       </c>
       <c r="G104" s="1">
         <v>12</v>
       </c>
       <c r="H104" s="16">
-        <f>ROUNDDOWN(((F104-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B105" s="1">
         <v>440</v>
       </c>
       <c r="F105" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2808</v>
       </c>
       <c r="G105" s="1">
         <v>12</v>
       </c>
       <c r="H105" s="16">
-        <f>ROUNDDOWN(((F105-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106" s="1">
         <v>480</v>
       </c>
       <c r="F106" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3630</v>
       </c>
       <c r="G106" s="1">
         <v>14</v>
       </c>
       <c r="H106" s="16">
-        <f>ROUNDDOWN(((F106-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107" s="1">
         <v>480</v>
       </c>
       <c r="F107" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3630</v>
       </c>
       <c r="G107" s="1">
         <v>14</v>
       </c>
       <c r="H107" s="16">
-        <f>ROUNDDOWN(((F107-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B108" s="1">
         <v>500</v>
       </c>
       <c r="F108" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3690</v>
       </c>
       <c r="G108" s="1">
         <v>16</v>
       </c>
       <c r="H108" s="16">
-        <f>ROUNDDOWN(((F108-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B109" s="1">
         <v>560</v>
       </c>
       <c r="F109" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>4257</v>
       </c>
       <c r="G109" s="1">
         <v>18</v>
       </c>
       <c r="H109" s="16">
-        <f>ROUNDDOWN(((F109-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>27</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B110" s="1">
         <v>620</v>
       </c>
       <c r="F110" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>4590</v>
       </c>
       <c r="G110" s="1">
         <v>20</v>
       </c>
       <c r="H110" s="16">
-        <f>ROUNDDOWN(((F110-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B111" s="1">
         <v>730</v>
       </c>
       <c r="F111" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>5256</v>
       </c>
       <c r="G111" s="1">
         <v>25</v>
       </c>
       <c r="H111" s="16">
-        <f>ROUNDDOWN(((F111-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="19"/>
         <v>34</v>
       </c>
     </row>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="113" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B113" s="1">
         <v>370</v>
@@ -2953,140 +2953,140 @@
         <v>0</v>
       </c>
       <c r="H113" s="16">
-        <f>ROUNDDOWN(((F113-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H113:H120" si="21">ROUNDDOWN(((F113-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B114" s="1">
         <v>410</v>
       </c>
       <c r="F114" s="1">
-        <f t="shared" ref="F114:F120" si="12">($E$112+B114)*(IF(B114&lt;=$C$8,1,0)*$D$8+IF(AND(B114&gt;$C$8,B114&lt;=$C$9),1,0)*$D$9+IF(AND(B114&gt;$C$9,B114&lt;=$C$10),1,0)*$D$10+IF(AND(B114&gt;$C$10,B114&lt;=$C$11),1,0)*$D$11+IF(AND(B114&gt;$C$11,B114&lt;=$C$12),1,0)*$D$12+IF(AND(B114&gt;$C$12,B114&lt;=$C$13),1,0)*$D$13+IF(AND(B114&gt;$C$13,B114&lt;=$C$14),1,0)*$D$14+IF(AND(B114&gt;$C$14,B114&lt;=$C$15),1,0)*$D$15+IF(AND(B114&gt;$C$15,B114&lt;=$C$16),1,0)*$D$16+IF(AND(B114&gt;$C$16,B114&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F114:F120" si="22">($E$112+B114)*(IF(B114&lt;=$C$8,1,0)*$D$8+IF(AND(B114&gt;$C$8,B114&lt;=$C$9),1,0)*$D$9+IF(AND(B114&gt;$C$9,B114&lt;=$C$10),1,0)*$D$10+IF(AND(B114&gt;$C$10,B114&lt;=$C$11),1,0)*$D$11+IF(AND(B114&gt;$C$11,B114&lt;=$C$12),1,0)*$D$12+IF(AND(B114&gt;$C$12,B114&lt;=$C$13),1,0)*$D$13+IF(AND(B114&gt;$C$13,B114&lt;=$C$14),1,0)*$D$14+IF(AND(B114&gt;$C$14,B114&lt;=$C$15),1,0)*$D$15+IF(AND(B114&gt;$C$15,B114&lt;=$C$16),1,0)*$D$16+IF(AND(B114&gt;$C$16,B114&lt;=$C$17),1,0)*$D$17)</f>
         <v>1824</v>
       </c>
       <c r="G114" s="1">
         <v>6</v>
       </c>
       <c r="H114" s="16">
-        <f>ROUNDDOWN(((F114-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B115" s="1">
         <v>450</v>
       </c>
       <c r="F115" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>2832</v>
       </c>
       <c r="G115" s="1">
         <v>10</v>
       </c>
       <c r="H115" s="16">
-        <f>ROUNDDOWN(((F115-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B116" s="1">
         <v>500</v>
       </c>
       <c r="F116" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>3690</v>
       </c>
       <c r="G116" s="1">
         <v>12</v>
       </c>
       <c r="H116" s="16">
-        <f>ROUNDDOWN(((F116-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>23</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B117" s="1">
         <v>520</v>
       </c>
       <c r="F117" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>4000</v>
       </c>
       <c r="G117" s="1">
         <v>15</v>
       </c>
       <c r="H117" s="16">
-        <f>ROUNDDOWN(((F117-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>26</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B118" s="1">
         <v>580</v>
       </c>
       <c r="F118" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>4323</v>
       </c>
       <c r="G118" s="1">
         <v>18</v>
       </c>
       <c r="H118" s="16">
-        <f>ROUNDDOWN(((F118-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>28</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B119" s="1">
         <v>650</v>
       </c>
       <c r="F119" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>4692</v>
       </c>
       <c r="G119" s="1">
         <v>20</v>
       </c>
       <c r="H119" s="16">
-        <f>ROUNDDOWN(((F119-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B120" s="1">
         <v>730</v>
       </c>
       <c r="F120" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>5256</v>
       </c>
       <c r="G120" s="1">
         <v>25</v>
       </c>
       <c r="H120" s="16">
-        <f>ROUNDDOWN(((F120-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="21"/>
         <v>34</v>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="122" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B122" s="1">
         <v>370</v>
@@ -3122,140 +3122,140 @@
         <v>0</v>
       </c>
       <c r="H122" s="16">
-        <f>ROUNDDOWN(((F122-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H122:H129" si="23">ROUNDDOWN(((F122-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B123" s="1">
         <v>410</v>
       </c>
       <c r="F123" s="1">
-        <f t="shared" ref="F123:F129" si="13">($E$121+B123)*(IF(B123&lt;=$C$8,1,0)*$D$8+IF(AND(B123&gt;$C$8,B123&lt;=$C$9),1,0)*$D$9+IF(AND(B123&gt;$C$9,B123&lt;=$C$10),1,0)*$D$10+IF(AND(B123&gt;$C$10,B123&lt;=$C$11),1,0)*$D$11+IF(AND(B123&gt;$C$11,B123&lt;=$C$12),1,0)*$D$12+IF(AND(B123&gt;$C$12,B123&lt;=$C$13),1,0)*$D$13+IF(AND(B123&gt;$C$13,B123&lt;=$C$14),1,0)*$D$14+IF(AND(B123&gt;$C$14,B123&lt;=$C$15),1,0)*$D$15+IF(AND(B123&gt;$C$15,B123&lt;=$C$16),1,0)*$D$16+IF(AND(B123&gt;$C$16,B123&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F123:F129" si="24">($E$121+B123)*(IF(B123&lt;=$C$8,1,0)*$D$8+IF(AND(B123&gt;$C$8,B123&lt;=$C$9),1,0)*$D$9+IF(AND(B123&gt;$C$9,B123&lt;=$C$10),1,0)*$D$10+IF(AND(B123&gt;$C$10,B123&lt;=$C$11),1,0)*$D$11+IF(AND(B123&gt;$C$11,B123&lt;=$C$12),1,0)*$D$12+IF(AND(B123&gt;$C$12,B123&lt;=$C$13),1,0)*$D$13+IF(AND(B123&gt;$C$13,B123&lt;=$C$14),1,0)*$D$14+IF(AND(B123&gt;$C$14,B123&lt;=$C$15),1,0)*$D$15+IF(AND(B123&gt;$C$15,B123&lt;=$C$16),1,0)*$D$16+IF(AND(B123&gt;$C$16,B123&lt;=$C$17),1,0)*$D$17)</f>
         <v>1824</v>
       </c>
       <c r="G123" s="1">
         <v>6</v>
       </c>
       <c r="H123" s="16">
-        <f>ROUNDDOWN(((F123-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B124" s="1">
         <v>450</v>
       </c>
       <c r="F124" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>2832</v>
       </c>
       <c r="G124" s="1">
         <v>10</v>
       </c>
       <c r="H124" s="16">
-        <f>ROUNDDOWN(((F124-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B125" s="1">
         <v>500</v>
       </c>
       <c r="F125" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>3690</v>
       </c>
       <c r="G125" s="1">
         <v>12</v>
       </c>
       <c r="H125" s="16">
-        <f>ROUNDDOWN(((F125-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>23</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" s="1">
         <v>520</v>
       </c>
       <c r="F126" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>4000</v>
       </c>
       <c r="G126" s="1">
         <v>15</v>
       </c>
       <c r="H126" s="16">
-        <f>ROUNDDOWN(((F126-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>26</v>
       </c>
     </row>
     <row r="127" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B127" s="1">
         <v>580</v>
       </c>
       <c r="F127" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>4323</v>
       </c>
       <c r="G127" s="1">
         <v>18</v>
       </c>
       <c r="H127" s="16">
-        <f>ROUNDDOWN(((F127-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B128" s="1">
         <v>650</v>
       </c>
       <c r="F128" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>4692</v>
       </c>
       <c r="G128" s="1">
         <v>20</v>
       </c>
       <c r="H128" s="16">
-        <f>ROUNDDOWN(((F128-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>30</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B129" s="1">
         <v>730</v>
       </c>
       <c r="F129" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>5256</v>
       </c>
       <c r="G129" s="1">
         <v>25</v>
       </c>
       <c r="H129" s="16">
-        <f>ROUNDDOWN(((F129-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="23"/>
         <v>34</v>
       </c>
     </row>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="131" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B131" s="1">
         <v>360</v>
@@ -3291,349 +3291,349 @@
         <v>0</v>
       </c>
       <c r="H131" s="16">
-        <f>ROUNDDOWN(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H131:H149" si="25">ROUNDDOWN(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B132" s="1">
         <v>370</v>
       </c>
       <c r="F132" s="1">
-        <f t="shared" ref="F132:F149" si="14">($E$130+B132)*(IF(B132&lt;=$C$8,1,0)*$D$8+IF(AND(B132&gt;$C$8,B132&lt;=$C$9),1,0)*$D$9+IF(AND(B132&gt;$C$9,B132&lt;=$C$10),1,0)*$D$10+IF(AND(B132&gt;$C$10,B132&lt;=$C$11),1,0)*$D$11+IF(AND(B132&gt;$C$11,B132&lt;=$C$12),1,0)*$D$12+IF(AND(B132&gt;$C$12,B132&lt;=$C$13),1,0)*$D$13+IF(AND(B132&gt;$C$13,B132&lt;=$C$14),1,0)*$D$14+IF(AND(B132&gt;$C$14,B132&lt;=$C$15),1,0)*$D$15+IF(AND(B132&gt;$C$15,B132&lt;=$C$16),1,0)*$D$16+IF(AND(B132&gt;$C$16,B132&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F132:F149" si="26">($E$130+B132)*(IF(B132&lt;=$C$8,1,0)*$D$8+IF(AND(B132&gt;$C$8,B132&lt;=$C$9),1,0)*$D$9+IF(AND(B132&gt;$C$9,B132&lt;=$C$10),1,0)*$D$10+IF(AND(B132&gt;$C$10,B132&lt;=$C$11),1,0)*$D$11+IF(AND(B132&gt;$C$11,B132&lt;=$C$12),1,0)*$D$12+IF(AND(B132&gt;$C$12,B132&lt;=$C$13),1,0)*$D$13+IF(AND(B132&gt;$C$13,B132&lt;=$C$14),1,0)*$D$14+IF(AND(B132&gt;$C$14,B132&lt;=$C$15),1,0)*$D$15+IF(AND(B132&gt;$C$15,B132&lt;=$C$16),1,0)*$D$16+IF(AND(B132&gt;$C$16,B132&lt;=$C$17),1,0)*$D$17)</f>
         <v>1760</v>
       </c>
       <c r="G132" s="1">
         <v>3</v>
       </c>
       <c r="H132" s="16">
-        <f>ROUNDDOWN(((F132-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B133" s="1">
         <v>380</v>
       </c>
       <c r="F133" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1776</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
       </c>
       <c r="H133" s="16">
-        <f>ROUNDDOWN(((F133-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B134" s="1">
         <v>400</v>
       </c>
       <c r="F134" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1808</v>
       </c>
       <c r="G134" s="1">
         <v>8</v>
       </c>
       <c r="H134" s="16">
-        <f>ROUNDDOWN(((F134-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B135" s="1">
         <v>410</v>
       </c>
       <c r="F135" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1824</v>
       </c>
       <c r="G135" s="1">
         <v>12</v>
       </c>
       <c r="H135" s="16">
-        <f>ROUNDDOWN(((F135-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B136" s="1">
         <v>420</v>
       </c>
       <c r="F136" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1840</v>
       </c>
       <c r="G136" s="1">
         <v>10</v>
       </c>
       <c r="H136" s="16">
-        <f>ROUNDDOWN(((F136-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B137" s="1">
         <v>440</v>
       </c>
       <c r="F137" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>2808</v>
       </c>
       <c r="G137" s="1">
         <v>12</v>
       </c>
       <c r="H137" s="16">
-        <f>ROUNDDOWN(((F137-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B138" s="1">
         <v>440</v>
       </c>
       <c r="F138" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>2808</v>
       </c>
       <c r="G138" s="1">
         <v>12</v>
       </c>
       <c r="H138" s="16">
-        <f>ROUNDDOWN(((F138-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B139" s="1">
         <v>450</v>
       </c>
       <c r="F139" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>2832</v>
       </c>
       <c r="G139" s="1">
         <v>14</v>
       </c>
       <c r="H139" s="16">
-        <f>ROUNDDOWN(((F139-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B140" s="1">
         <v>480</v>
       </c>
       <c r="F140" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>3630</v>
       </c>
       <c r="G140" s="1">
         <v>14</v>
       </c>
       <c r="H140" s="16">
-        <f>ROUNDDOWN(((F140-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>23</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B141" s="1">
         <v>480</v>
       </c>
       <c r="F141" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>3630</v>
       </c>
       <c r="G141" s="1">
         <v>14</v>
       </c>
       <c r="H141" s="16">
-        <f>ROUNDDOWN(((F141-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>23</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B142" s="1">
         <v>490</v>
       </c>
       <c r="F142" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>3660</v>
       </c>
       <c r="G142" s="1">
         <v>15</v>
       </c>
       <c r="H142" s="16">
-        <f>ROUNDDOWN(((F142-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>23</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B143" s="1">
         <v>500</v>
       </c>
       <c r="F143" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>3690</v>
       </c>
       <c r="G143" s="1">
         <v>16</v>
       </c>
       <c r="H143" s="16">
-        <f>ROUNDDOWN(((F143-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>23</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B144" s="1">
         <v>520</v>
       </c>
       <c r="F144" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>4000</v>
       </c>
       <c r="G144" s="1">
         <v>17</v>
       </c>
       <c r="H144" s="16">
-        <f>ROUNDDOWN(((F144-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>26</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B145" s="1">
         <v>560</v>
       </c>
       <c r="F145" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>4257</v>
       </c>
       <c r="G145" s="1">
         <v>18</v>
       </c>
       <c r="H145" s="16">
-        <f>ROUNDDOWN(((F145-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>27</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B146" s="1">
         <v>580</v>
       </c>
       <c r="F146" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>4323</v>
       </c>
       <c r="G146" s="1">
         <v>18</v>
       </c>
       <c r="H146" s="16">
-        <f>ROUNDDOWN(((F146-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>28</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B147" s="1">
         <v>620</v>
       </c>
       <c r="F147" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>4590</v>
       </c>
       <c r="G147" s="1">
         <v>20</v>
       </c>
       <c r="H147" s="16">
-        <f>ROUNDDOWN(((F147-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>30</v>
       </c>
     </row>
     <row r="148" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B148" s="1">
         <v>730</v>
       </c>
       <c r="F148" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>5256</v>
       </c>
       <c r="G148" s="1">
         <v>24</v>
       </c>
       <c r="H148" s="16">
-        <f>ROUNDDOWN(((F148-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>34</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B149" s="1">
         <v>730</v>
       </c>
       <c r="F149" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>5256</v>
       </c>
       <c r="G149" s="1">
         <v>25</v>
       </c>
       <c r="H149" s="16">
-        <f>ROUNDDOWN(((F149-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="25"/>
         <v>34</v>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="151" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B151" s="1">
         <v>540</v>
@@ -3675,13 +3675,13 @@
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B152" s="1">
         <v>600</v>
       </c>
       <c r="F152" s="1">
-        <f t="shared" ref="F152:F154" si="15">($E$150+B152)*(IF(B152&lt;=$C$8,1,0)*$D$8+IF(AND(B152&gt;$C$8,B152&lt;=$C$9),1,0)*$D$9+IF(AND(B152&gt;$C$9,B152&lt;=$C$10),1,0)*$D$10+IF(AND(B152&gt;$C$10,B152&lt;=$C$11),1,0)*$D$11+IF(AND(B152&gt;$C$11,B152&lt;=$C$12),1,0)*$D$12+IF(AND(B152&gt;$C$12,B152&lt;=$C$13),1,0)*$D$13+IF(AND(B152&gt;$C$13,B152&lt;=$C$14),1,0)*$D$14+IF(AND(B152&gt;$C$14,B152&lt;=$C$15),1,0)*$D$15+IF(AND(B152&gt;$C$15,B152&lt;=$C$16),1,0)*$D$16+IF(AND(B152&gt;$C$16,B152&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F152:F154" si="27">($E$150+B152)*(IF(B152&lt;=$C$8,1,0)*$D$8+IF(AND(B152&gt;$C$8,B152&lt;=$C$9),1,0)*$D$9+IF(AND(B152&gt;$C$9,B152&lt;=$C$10),1,0)*$D$10+IF(AND(B152&gt;$C$10,B152&lt;=$C$11),1,0)*$D$11+IF(AND(B152&gt;$C$11,B152&lt;=$C$12),1,0)*$D$12+IF(AND(B152&gt;$C$12,B152&lt;=$C$13),1,0)*$D$13+IF(AND(B152&gt;$C$13,B152&lt;=$C$14),1,0)*$D$14+IF(AND(B152&gt;$C$14,B152&lt;=$C$15),1,0)*$D$15+IF(AND(B152&gt;$C$15,B152&lt;=$C$16),1,0)*$D$16+IF(AND(B152&gt;$C$16,B152&lt;=$C$17),1,0)*$D$17)</f>
         <v>4455</v>
       </c>
       <c r="G152" s="1">
@@ -3694,13 +3694,13 @@
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B153" s="1">
         <v>700</v>
       </c>
       <c r="F153" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="27"/>
         <v>5075</v>
       </c>
       <c r="G153" s="1">
@@ -3713,13 +3713,13 @@
     </row>
     <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B154" s="1">
         <v>750</v>
       </c>
       <c r="F154" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="27"/>
         <v>5400</v>
       </c>
       <c r="G154" s="1">
@@ -3749,7 +3749,7 @@
     </row>
     <row r="156" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B156" s="1">
         <v>420</v>
@@ -3762,159 +3762,159 @@
         <v>0</v>
       </c>
       <c r="H156" s="16">
-        <f>ROUNDDOWN(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H156:H164" si="28">ROUNDDOWN(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B157" s="1">
         <v>460</v>
       </c>
       <c r="F157" s="1">
-        <f t="shared" ref="F157:F164" si="16">($E$155+B157)*(IF(B157&lt;=$C$8,1,0)*$D$8+IF(AND(B157&gt;$C$8,B157&lt;=$C$9),1,0)*$D$9+IF(AND(B157&gt;$C$9,B157&lt;=$C$10),1,0)*$D$10+IF(AND(B157&gt;$C$10,B157&lt;=$C$11),1,0)*$D$11+IF(AND(B157&gt;$C$11,B157&lt;=$C$12),1,0)*$D$12+IF(AND(B157&gt;$C$12,B157&lt;=$C$13),1,0)*$D$13+IF(AND(B157&gt;$C$13,B157&lt;=$C$14),1,0)*$D$14+IF(AND(B157&gt;$C$14,B157&lt;=$C$15),1,0)*$D$15+IF(AND(B157&gt;$C$15,B157&lt;=$C$16),1,0)*$D$16+IF(AND(B157&gt;$C$16,B157&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F157:F164" si="29">($E$155+B157)*(IF(B157&lt;=$C$8,1,0)*$D$8+IF(AND(B157&gt;$C$8,B157&lt;=$C$9),1,0)*$D$9+IF(AND(B157&gt;$C$9,B157&lt;=$C$10),1,0)*$D$10+IF(AND(B157&gt;$C$10,B157&lt;=$C$11),1,0)*$D$11+IF(AND(B157&gt;$C$11,B157&lt;=$C$12),1,0)*$D$12+IF(AND(B157&gt;$C$12,B157&lt;=$C$13),1,0)*$D$13+IF(AND(B157&gt;$C$13,B157&lt;=$C$14),1,0)*$D$14+IF(AND(B157&gt;$C$14,B157&lt;=$C$15),1,0)*$D$15+IF(AND(B157&gt;$C$15,B157&lt;=$C$16),1,0)*$D$16+IF(AND(B157&gt;$C$16,B157&lt;=$C$17),1,0)*$D$17)</f>
         <v>3630</v>
       </c>
       <c r="G157" s="1">
         <v>0</v>
       </c>
       <c r="H157" s="16">
-        <f>ROUNDDOWN(((F157-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>23</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B158" s="1">
         <v>460</v>
       </c>
       <c r="F158" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>3630</v>
       </c>
       <c r="G158" s="1">
         <v>2</v>
       </c>
       <c r="H158" s="16">
-        <f>ROUNDDOWN(((F158-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>23</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B159" s="1">
         <v>500</v>
       </c>
       <c r="F159" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>3750</v>
       </c>
       <c r="G159" s="1">
         <v>6</v>
       </c>
       <c r="H159" s="16">
-        <f>ROUNDDOWN(((F159-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B160" s="1">
         <v>540</v>
       </c>
       <c r="F160" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>4128</v>
       </c>
       <c r="G160" s="1">
         <v>6</v>
       </c>
       <c r="H160" s="16">
-        <f>ROUNDDOWN(((F160-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>26</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B161" s="1">
         <v>540</v>
       </c>
       <c r="F161" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>4128</v>
       </c>
       <c r="G161" s="1">
         <v>11</v>
       </c>
       <c r="H161" s="16">
-        <f>ROUNDDOWN(((F161-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>26</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B162" s="1">
         <v>600</v>
       </c>
       <c r="F162" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>4455</v>
       </c>
       <c r="G162" s="1">
         <v>10</v>
       </c>
       <c r="H162" s="16">
-        <f>ROUNDDOWN(((F162-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B163" s="1">
         <v>700</v>
       </c>
       <c r="F163" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>5075</v>
       </c>
       <c r="G163" s="1">
         <v>16</v>
       </c>
       <c r="H163" s="16">
-        <f>ROUNDDOWN(((F163-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>33</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B164" s="1">
         <v>750</v>
       </c>
       <c r="F164" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>5400</v>
       </c>
       <c r="G164" s="1">
         <v>16</v>
       </c>
       <c r="H164" s="16">
-        <f>ROUNDDOWN(((F164-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="28"/>
         <v>36</v>
       </c>
     </row>

</xml_diff>